<commit_message>
Added a file I forgot to commit
</commit_message>
<xml_diff>
--- a/exports/yield_files/USB Oil 5 Late.xlsx
+++ b/exports/yield_files/USB Oil 5 Late.xlsx
@@ -552,9 +552,15 @@
       <c r="N2" t="n">
         <v>3</v>
       </c>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
+      <c r="O2" t="n">
+        <v>22.79</v>
+      </c>
+      <c r="P2" t="n">
+        <v>43.07</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>65.86</v>
+      </c>
       <c r="R2" t="n">
         <v>1893.1</v>
       </c>
@@ -605,9 +611,15 @@
       <c r="N3" t="n">
         <v>2</v>
       </c>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
+      <c r="O3" t="n">
+        <v>22.94</v>
+      </c>
+      <c r="P3" t="n">
+        <v>43.28</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>66.22</v>
+      </c>
       <c r="R3" t="n">
         <v>1758</v>
       </c>
@@ -652,9 +664,15 @@
       </c>
       <c r="M4"/>
       <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
+      <c r="O4" t="n">
+        <v>22.67</v>
+      </c>
+      <c r="P4" t="n">
+        <v>42.87</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>65.54</v>
+      </c>
       <c r="R4" t="n">
         <v>1686.3</v>
       </c>
@@ -701,9 +719,15 @@
       <c r="N5" t="n">
         <v>1.5</v>
       </c>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
+      <c r="O5" t="n">
+        <v>23.46</v>
+      </c>
+      <c r="P5" t="n">
+        <v>40.66</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>64.12</v>
+      </c>
       <c r="R5" t="n">
         <v>1570.5</v>
       </c>
@@ -754,9 +778,15 @@
       <c r="N6" t="n">
         <v>1</v>
       </c>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
+      <c r="O6" t="n">
+        <v>24.16</v>
+      </c>
+      <c r="P6" t="n">
+        <v>39.73</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>63.89</v>
+      </c>
       <c r="R6" t="n">
         <v>2130.5</v>
       </c>
@@ -801,9 +831,15 @@
       </c>
       <c r="M7"/>
       <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
+      <c r="O7" t="n">
+        <v>24.09</v>
+      </c>
+      <c r="P7" t="n">
+        <v>39.17</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>63.26</v>
+      </c>
       <c r="R7" t="n">
         <v>2439.2</v>
       </c>
@@ -850,9 +886,15 @@
       <c r="N8" t="n">
         <v>1.5</v>
       </c>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
+      <c r="O8" t="n">
+        <v>22.44</v>
+      </c>
+      <c r="P8" t="n">
+        <v>42.75</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>65.19</v>
+      </c>
       <c r="R8" t="n">
         <v>2385.6</v>
       </c>
@@ -903,9 +945,15 @@
       <c r="N9" t="n">
         <v>1.5</v>
       </c>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
+      <c r="O9" t="n">
+        <v>22.9</v>
+      </c>
+      <c r="P9" t="n">
+        <v>42.18</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>65.08</v>
+      </c>
       <c r="R9" t="n">
         <v>2221.8</v>
       </c>
@@ -950,9 +998,15 @@
       </c>
       <c r="M10"/>
       <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
+      <c r="O10" t="n">
+        <v>22.36</v>
+      </c>
+      <c r="P10" t="n">
+        <v>43.28</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>65.64</v>
+      </c>
       <c r="R10" t="n">
         <v>2454.9</v>
       </c>
@@ -999,9 +1053,15 @@
       <c r="N11" t="n">
         <v>1</v>
       </c>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
+      <c r="O11" t="n">
+        <v>23.96</v>
+      </c>
+      <c r="P11" t="n">
+        <v>41.26</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>65.22</v>
+      </c>
       <c r="R11" t="n">
         <v>2046</v>
       </c>
@@ -1052,9 +1112,15 @@
       <c r="N12" t="n">
         <v>1</v>
       </c>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
+      <c r="O12" t="n">
+        <v>24.01</v>
+      </c>
+      <c r="P12" t="n">
+        <v>41.86</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>65.87</v>
+      </c>
       <c r="R12" t="n">
         <v>2014.2</v>
       </c>
@@ -1099,9 +1165,15 @@
       </c>
       <c r="M13"/>
       <c r="N13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
+      <c r="O13" t="n">
+        <v>23.28</v>
+      </c>
+      <c r="P13" t="n">
+        <v>41.37</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>64.65</v>
+      </c>
       <c r="R13" t="n">
         <v>2080.1</v>
       </c>
@@ -1148,9 +1220,15 @@
       <c r="N14" t="n">
         <v>2</v>
       </c>
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
+      <c r="O14" t="n">
+        <v>22.77</v>
+      </c>
+      <c r="P14" t="n">
+        <v>43.42</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>66.19</v>
+      </c>
       <c r="R14" t="n">
         <v>1660.9</v>
       </c>
@@ -1201,9 +1279,15 @@
       <c r="N15" t="n">
         <v>1.5</v>
       </c>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
+      <c r="O15" t="n">
+        <v>22.89</v>
+      </c>
+      <c r="P15" t="n">
+        <v>41.81</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>64.7</v>
+      </c>
       <c r="R15" t="n">
         <v>1728.3</v>
       </c>
@@ -1248,9 +1332,15 @@
       </c>
       <c r="M16"/>
       <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
+      <c r="O16" t="n">
+        <v>22.82</v>
+      </c>
+      <c r="P16" t="n">
+        <v>43.62</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>66.44</v>
+      </c>
       <c r="R16" t="n">
         <v>2136</v>
       </c>
@@ -1297,9 +1387,15 @@
       <c r="N17" t="n">
         <v>2</v>
       </c>
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
+      <c r="O17" t="n">
+        <v>23.22</v>
+      </c>
+      <c r="P17" t="n">
+        <v>42.83</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>66.05</v>
+      </c>
       <c r="R17" t="n">
         <v>1725.8</v>
       </c>
@@ -1350,9 +1446,15 @@
       <c r="N18" t="n">
         <v>1.5</v>
       </c>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
+      <c r="O18" t="n">
+        <v>22.87</v>
+      </c>
+      <c r="P18" t="n">
+        <v>43.54</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>66.41</v>
+      </c>
       <c r="R18" t="n">
         <v>2275.2</v>
       </c>
@@ -1397,9 +1499,15 @@
       </c>
       <c r="M19"/>
       <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
+      <c r="O19" t="n">
+        <v>23.35</v>
+      </c>
+      <c r="P19" t="n">
+        <v>42.75</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>66.1</v>
+      </c>
       <c r="R19" t="n">
         <v>2025.3</v>
       </c>
@@ -1448,9 +1556,15 @@
       <c r="N20" t="n">
         <v>1</v>
       </c>
-      <c r="O20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
+      <c r="O20" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="P20" t="n">
+        <v>45.65</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>67.75</v>
+      </c>
       <c r="R20" t="n">
         <v>1726.1</v>
       </c>
@@ -1501,9 +1615,15 @@
       <c r="N21" t="n">
         <v>1</v>
       </c>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
+      <c r="O21" t="n">
+        <v>21.49</v>
+      </c>
+      <c r="P21" t="n">
+        <v>45.4</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>66.89</v>
+      </c>
       <c r="R21" t="n">
         <v>1483.6</v>
       </c>
@@ -1548,9 +1668,15 @@
       </c>
       <c r="M22"/>
       <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
+      <c r="O22" t="n">
+        <v>20.95</v>
+      </c>
+      <c r="P22" t="n">
+        <v>45.42</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>66.37</v>
+      </c>
       <c r="R22" t="n">
         <v>1999.4</v>
       </c>
@@ -1597,9 +1723,15 @@
       <c r="N23" t="n">
         <v>1</v>
       </c>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
+      <c r="O23" t="n">
+        <v>23.62</v>
+      </c>
+      <c r="P23" t="n">
+        <v>40.69</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>64.31</v>
+      </c>
       <c r="R23" t="n">
         <v>1835.8</v>
       </c>
@@ -1650,9 +1782,15 @@
       <c r="N24" t="n">
         <v>1.5</v>
       </c>
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
+      <c r="O24" t="n">
+        <v>24.27</v>
+      </c>
+      <c r="P24" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>63.47</v>
+      </c>
       <c r="R24" t="n">
         <v>2139</v>
       </c>
@@ -1697,9 +1835,15 @@
       </c>
       <c r="M25"/>
       <c r="N25"/>
-      <c r="O25"/>
-      <c r="P25"/>
-      <c r="Q25"/>
+      <c r="O25" t="n">
+        <v>23.71</v>
+      </c>
+      <c r="P25" t="n">
+        <v>39.41</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>63.12</v>
+      </c>
       <c r="R25" t="n">
         <v>1994.6</v>
       </c>

</xml_diff>